<commit_message>
Edit owner and due dates of tasks
</commit_message>
<xml_diff>
--- a/Project551.xlsx
+++ b/Project551.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB33CCDD-E9DF-43A7-AE46-D3190D39BEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B721A-C988-4D0F-A1AA-B836DA5784B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Activity</t>
   </si>
@@ -112,25 +112,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Team work contract
-team-contract.md</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CODE_OF_CONDUCT.md</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>A statement on inclusivity and harassment free involvement in the project.
-Details on expected behaviour and unacceptable behaviour.
-A procedure for reporting unacceptable behaviour.</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CONTRIBUTING.md</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>README.md</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -142,10 +123,6 @@
   <si>
     <t>Distribute Jobs for Milestone1
 Discuss Team Work Contrat</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Preparation</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -162,28 +139,60 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Section 2: Description of the data</t>
+    <t>proposal.md
+Section 1: Motivation and Purpose
+Section 2: Description of the data
+Section 3: Research questions and usage scenarios</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Section 3: Research questions and usage scenarios</t>
+    <t xml:space="preserve">Proposal </t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Proposal -1</t>
+    <t>Ricky</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>proposal.md
-Section 1: Motivation and Purpose</t>
+    <t>Madison</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Proposal -2</t>
+    <t>Sophie</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Proposal -3</t>
+    <t>1. CONTRIBUTING.md
+2. team-contract.md
+2. CODE_OF_CONDUCT.md</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agreements</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start developing your app (Optional)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Everyone</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstorming</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ricky, Sophie</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madison, Sophie</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ricky, Madison</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -741,94 +750,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>44973</c:v>
+                  <c:v>44975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44974</c:v>
+                  <c:v>44976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44975</c:v>
+                  <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44976</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44977</c:v>
+                  <c:v>44979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44978</c:v>
+                  <c:v>44980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44979</c:v>
+                  <c:v>44981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44980</c:v>
+                  <c:v>44982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44981</c:v>
+                  <c:v>44983</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44982</c:v>
+                  <c:v>44984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44983</c:v>
+                  <c:v>44985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44984</c:v>
+                  <c:v>44986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44985</c:v>
+                  <c:v>44987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44986</c:v>
+                  <c:v>44988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44987</c:v>
+                  <c:v>44989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44988</c:v>
+                  <c:v>44990</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44989</c:v>
+                  <c:v>44991</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44990</c:v>
+                  <c:v>44992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44991</c:v>
+                  <c:v>44993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44992</c:v>
+                  <c:v>44994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44993</c:v>
+                  <c:v>44995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44994</c:v>
+                  <c:v>44996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44995</c:v>
+                  <c:v>44997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44996</c:v>
+                  <c:v>44998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44997</c:v>
+                  <c:v>44999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44998</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44999</c:v>
+                  <c:v>45001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45000</c:v>
+                  <c:v>45002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45001</c:v>
+                  <c:v>45003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45002</c:v>
+                  <c:v>45004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -840,13 +849,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>11.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -948,7 +957,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PREPARATION</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1002,7 +1011,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1135,94 +1144,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>44973</c:v>
+                  <c:v>44975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44974</c:v>
+                  <c:v>44976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44975</c:v>
+                  <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44976</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44977</c:v>
+                  <c:v>44979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44978</c:v>
+                  <c:v>44980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44979</c:v>
+                  <c:v>44981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44980</c:v>
+                  <c:v>44982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44981</c:v>
+                  <c:v>44983</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44982</c:v>
+                  <c:v>44984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44983</c:v>
+                  <c:v>44985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44984</c:v>
+                  <c:v>44986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44985</c:v>
+                  <c:v>44987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44986</c:v>
+                  <c:v>44988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44987</c:v>
+                  <c:v>44989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44988</c:v>
+                  <c:v>44990</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44989</c:v>
+                  <c:v>44991</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44990</c:v>
+                  <c:v>44992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44991</c:v>
+                  <c:v>44993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44992</c:v>
+                  <c:v>44994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44993</c:v>
+                  <c:v>44995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44994</c:v>
+                  <c:v>44996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44995</c:v>
+                  <c:v>44997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44996</c:v>
+                  <c:v>44998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44997</c:v>
+                  <c:v>44999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44998</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44999</c:v>
+                  <c:v>45001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45000</c:v>
+                  <c:v>45002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45001</c:v>
+                  <c:v>45003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45002</c:v>
+                  <c:v>45004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,7 +1249,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1342,7 +1351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FIRST MEETING</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1396,7 +1405,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1529,94 +1538,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>44973</c:v>
+                  <c:v>44975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44974</c:v>
+                  <c:v>44976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44975</c:v>
+                  <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44976</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44977</c:v>
+                  <c:v>44979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44978</c:v>
+                  <c:v>44980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44979</c:v>
+                  <c:v>44981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44980</c:v>
+                  <c:v>44982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44981</c:v>
+                  <c:v>44983</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44982</c:v>
+                  <c:v>44984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44983</c:v>
+                  <c:v>44985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44984</c:v>
+                  <c:v>44986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44985</c:v>
+                  <c:v>44987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44986</c:v>
+                  <c:v>44988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44987</c:v>
+                  <c:v>44989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44988</c:v>
+                  <c:v>44990</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44989</c:v>
+                  <c:v>44991</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44990</c:v>
+                  <c:v>44992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44991</c:v>
+                  <c:v>44993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44992</c:v>
+                  <c:v>44994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44993</c:v>
+                  <c:v>44995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44994</c:v>
+                  <c:v>44996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44995</c:v>
+                  <c:v>44997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44996</c:v>
+                  <c:v>44998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44997</c:v>
+                  <c:v>44999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44998</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44999</c:v>
+                  <c:v>45001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45000</c:v>
+                  <c:v>45002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45001</c:v>
+                  <c:v>45003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45002</c:v>
+                  <c:v>45004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1637,13 +1646,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -1736,7 +1745,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PROPOSAL -1</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1802,7 +1811,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -1932,94 +1941,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>44973</c:v>
+                  <c:v>44975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44974</c:v>
+                  <c:v>44976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44975</c:v>
+                  <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44976</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44977</c:v>
+                  <c:v>44979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44978</c:v>
+                  <c:v>44980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44979</c:v>
+                  <c:v>44981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44980</c:v>
+                  <c:v>44982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44981</c:v>
+                  <c:v>44983</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44982</c:v>
+                  <c:v>44984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44983</c:v>
+                  <c:v>44985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44984</c:v>
+                  <c:v>44986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44985</c:v>
+                  <c:v>44987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44986</c:v>
+                  <c:v>44988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44987</c:v>
+                  <c:v>44989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44988</c:v>
+                  <c:v>44990</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44989</c:v>
+                  <c:v>44991</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44990</c:v>
+                  <c:v>44992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44991</c:v>
+                  <c:v>44993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44992</c:v>
+                  <c:v>44994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44993</c:v>
+                  <c:v>44995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44994</c:v>
+                  <c:v>44996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44995</c:v>
+                  <c:v>44997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44996</c:v>
+                  <c:v>44998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44997</c:v>
+                  <c:v>44999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44998</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44999</c:v>
+                  <c:v>45001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45000</c:v>
+                  <c:v>45002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45001</c:v>
+                  <c:v>45003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45002</c:v>
+                  <c:v>45004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2031,7 +2040,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2040,13 +2049,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2139,7 +2148,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PROPOSAL -2</c:v>
+                  <c:v>BRAINSTORMING</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2187,7 +2196,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2202,7 +2211,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2326,94 +2335,94 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>44973</c:v>
+                  <c:v>44975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44974</c:v>
+                  <c:v>44976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44975</c:v>
+                  <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44976</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44977</c:v>
+                  <c:v>44979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44978</c:v>
+                  <c:v>44980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44979</c:v>
+                  <c:v>44981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44980</c:v>
+                  <c:v>44982</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44981</c:v>
+                  <c:v>44983</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44982</c:v>
+                  <c:v>44984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44983</c:v>
+                  <c:v>44985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44984</c:v>
+                  <c:v>44986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44985</c:v>
+                  <c:v>44987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44986</c:v>
+                  <c:v>44988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44987</c:v>
+                  <c:v>44989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44988</c:v>
+                  <c:v>44990</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44989</c:v>
+                  <c:v>44991</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44990</c:v>
+                  <c:v>44992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44991</c:v>
+                  <c:v>44993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44992</c:v>
+                  <c:v>44994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44993</c:v>
+                  <c:v>44995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44994</c:v>
+                  <c:v>44996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44995</c:v>
+                  <c:v>44997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44996</c:v>
+                  <c:v>44998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44997</c:v>
+                  <c:v>44999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44998</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44999</c:v>
+                  <c:v>45001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45000</c:v>
+                  <c:v>45002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45001</c:v>
+                  <c:v>45003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45002</c:v>
+                  <c:v>45004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,7 +2434,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>7.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2434,13 +2443,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2533,7 +2542,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PROPOSAL -3</c:v>
+                  <c:v>FIRST MEETING</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2626,7 +2635,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>7.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2641,7 +2650,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2757,22 +2766,22 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>6.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>6.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>6.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>#N/A</c:v>
@@ -2862,7 +2871,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>README.MD</c:v>
+                  <c:v>PROPOSAL </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2936,7 +2945,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>6.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -2945,7 +2954,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>#N/A</c:v>
@@ -3065,19 +3074,19 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>1.7666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3170,8 +3179,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TEAM WORK CONTRACT
-TEAM-CONTRACT.MD</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3248,10 +3256,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3380,13 +3388,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3479,7 +3487,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CODE_OF_CONDUCT.MD</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3559,7 +3567,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3688,13 +3696,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3787,7 +3795,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CONTRIBUTING.MD</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3867,7 +3875,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -4149,10 +4157,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -4282,10 +4290,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.5</c:v>
@@ -4444,13 +4452,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>#N/A</c:v>
@@ -4751,7 +4759,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>16</c:v>
+                      <c:v>18</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4767,12 +4775,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{687E8CD8-7585-4C17-9F3C-6936B7912CAB}</c15:txfldGUID>
+                      <c15:txfldGUID>{2C7EF9C8-F2C2-4966-9F4F-AE2D539DE26B}</c15:txfldGUID>
                       <c15:f>calcs!$E$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>16</c:v>
+                          <c:v>18</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4792,7 +4800,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>17</c:v>
+                      <c:v>19</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4808,12 +4816,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A50D32DC-A401-4F0D-8FAD-81AA2C9D738A}</c15:txfldGUID>
+                      <c15:txfldGUID>{64FC1BD5-515D-4A36-BFFA-CA9F607CCA3A}</c15:txfldGUID>
                       <c15:f>calcs!$F$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>17</c:v>
+                          <c:v>19</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4833,7 +4841,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>18</c:v>
+                      <c:v>20</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4849,12 +4857,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{89CE7E78-8940-464A-AB30-85E129184D89}</c15:txfldGUID>
+                      <c15:txfldGUID>{71EF8B9E-24C1-4C1E-88B6-001C405F3B06}</c15:txfldGUID>
                       <c15:f>calcs!$G$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>18</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4874,7 +4882,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>19</c:v>
+                      <c:v>21</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4890,12 +4898,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{606DE13A-2B82-49AF-930A-25E3B3365474}</c15:txfldGUID>
+                      <c15:txfldGUID>{9EFE8699-4E9F-49E2-A0F0-763D15235BC8}</c15:txfldGUID>
                       <c15:f>calcs!$H$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>19</c:v>
+                          <c:v>21</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4915,7 +4923,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>20</c:v>
+                      <c:v>22</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4931,12 +4939,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8EE8EAFF-3A68-4C8C-B451-A2CD15109290}</c15:txfldGUID>
+                      <c15:txfldGUID>{D4F008DF-355C-4929-990D-720B97C86007}</c15:txfldGUID>
                       <c15:f>calcs!$I$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>20</c:v>
+                          <c:v>22</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4956,7 +4964,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>21</c:v>
+                      <c:v>23</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -4972,12 +4980,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0C77A53D-25BF-465D-9399-FFB7D20387F0}</c15:txfldGUID>
+                      <c15:txfldGUID>{1A78D3C4-F44F-4F27-9D88-A6C30EC09F02}</c15:txfldGUID>
                       <c15:f>calcs!$J$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>21</c:v>
+                          <c:v>23</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -4997,7 +5005,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>22</c:v>
+                      <c:v>24</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5013,12 +5021,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8FC27751-D6D6-46B1-AAF6-E1DC990A3717}</c15:txfldGUID>
+                      <c15:txfldGUID>{E6ED9076-5A0E-4775-9474-7DFF0CCF48CA}</c15:txfldGUID>
                       <c15:f>calcs!$K$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>22</c:v>
+                          <c:v>24</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5038,7 +5046,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>23</c:v>
+                      <c:v>25</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5054,12 +5062,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D0A6C13B-FD30-4315-908F-A08D334ED14A}</c15:txfldGUID>
+                      <c15:txfldGUID>{BDFCABED-7DDE-4D20-B6ED-E1B6BB0661E3}</c15:txfldGUID>
                       <c15:f>calcs!$L$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>23</c:v>
+                          <c:v>25</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5079,7 +5087,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>24</c:v>
+                      <c:v>26</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5095,12 +5103,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{34369716-1E7C-4540-83A4-B31F7E3ED717}</c15:txfldGUID>
+                      <c15:txfldGUID>{248953C1-19EF-4669-9755-B0BD528E5353}</c15:txfldGUID>
                       <c15:f>calcs!$M$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>24</c:v>
+                          <c:v>26</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5120,7 +5128,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>25</c:v>
+                      <c:v>27</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5136,12 +5144,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7ADC2051-27D3-42B0-85B0-A6C09D193994}</c15:txfldGUID>
+                      <c15:txfldGUID>{70F73F8E-76D7-4069-84A8-4FF0FBBFDC33}</c15:txfldGUID>
                       <c15:f>calcs!$N$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>25</c:v>
+                          <c:v>27</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5161,7 +5169,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>26</c:v>
+                      <c:v>28</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5177,12 +5185,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{241D4D1D-1546-4934-856C-29D35EEAE8E1}</c15:txfldGUID>
+                      <c15:txfldGUID>{875820C8-5C18-4681-8AEB-921AE6CC5347}</c15:txfldGUID>
                       <c15:f>calcs!$O$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>26</c:v>
+                          <c:v>28</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5202,7 +5210,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>27</c:v>
+                      <c:v>01</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5218,12 +5226,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D729E74A-C2E7-4433-A929-7EDFC78F7A6A}</c15:txfldGUID>
+                      <c15:txfldGUID>{623ECE00-4E02-466F-B07C-849418F2A1C2}</c15:txfldGUID>
                       <c15:f>calcs!$P$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>27</c:v>
+                          <c:v>01</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5243,7 +5251,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>28</c:v>
+                      <c:v>02</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5259,12 +5267,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2EB533E4-7A31-44E0-A5F8-219956EEC036}</c15:txfldGUID>
+                      <c15:txfldGUID>{007A141F-5C08-457E-8BA6-C490AE0A2C6A}</c15:txfldGUID>
                       <c15:f>calcs!$Q$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>28</c:v>
+                          <c:v>02</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5284,7 +5292,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>01</c:v>
+                      <c:v>03</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5300,12 +5308,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FE48CDF9-7E55-4008-999F-D3D753045FA0}</c15:txfldGUID>
+                      <c15:txfldGUID>{B653C953-EA84-4096-9777-9522B292C3D0}</c15:txfldGUID>
                       <c15:f>calcs!$R$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>01</c:v>
+                          <c:v>03</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5325,7 +5333,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>02</c:v>
+                      <c:v>04</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5341,12 +5349,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DE345A8B-CEF5-49FF-907F-93857E19DD97}</c15:txfldGUID>
+                      <c15:txfldGUID>{7CA2E3A5-D6D0-47D4-8A5D-68741EC2E109}</c15:txfldGUID>
                       <c15:f>calcs!$S$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>02</c:v>
+                          <c:v>04</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5366,7 +5374,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>03</c:v>
+                      <c:v>05</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5382,12 +5390,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{800ED701-AE6B-42FE-85DF-A5D93DCE01C4}</c15:txfldGUID>
+                      <c15:txfldGUID>{43D52BC7-D155-46A1-B0FD-E8F5FA75D20D}</c15:txfldGUID>
                       <c15:f>calcs!$T$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>03</c:v>
+                          <c:v>05</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5407,7 +5415,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>04</c:v>
+                      <c:v>06</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5423,12 +5431,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C804A181-E1CF-49F9-8B9F-C646F3381CA1}</c15:txfldGUID>
+                      <c15:txfldGUID>{B32D43DD-207F-4A3C-A2D8-93545FD050C6}</c15:txfldGUID>
                       <c15:f>calcs!$U$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>04</c:v>
+                          <c:v>06</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5448,7 +5456,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>05</c:v>
+                      <c:v>07</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5464,12 +5472,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{626BD9C6-9480-47E3-9B03-B3CC78F3FEFA}</c15:txfldGUID>
+                      <c15:txfldGUID>{663CA20C-A1F5-420A-8D56-EEE414895C32}</c15:txfldGUID>
                       <c15:f>calcs!$V$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>05</c:v>
+                          <c:v>07</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5489,7 +5497,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>06</c:v>
+                      <c:v>08</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5505,12 +5513,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AD7ED610-A60F-41B1-B32D-EA9A4B4F63A5}</c15:txfldGUID>
+                      <c15:txfldGUID>{7075CBDD-22A8-496A-8C62-7AAADC648BE1}</c15:txfldGUID>
                       <c15:f>calcs!$W$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>06</c:v>
+                          <c:v>08</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5530,7 +5538,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>07</c:v>
+                      <c:v>09</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5546,12 +5554,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{479A2B8C-15BC-448B-8BA5-F019E02D15CF}</c15:txfldGUID>
+                      <c15:txfldGUID>{62F991BB-6EBC-4B48-99A9-A9037AC53078}</c15:txfldGUID>
                       <c15:f>calcs!$X$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>07</c:v>
+                          <c:v>09</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5571,7 +5579,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>08</c:v>
+                      <c:v>10</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5587,12 +5595,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0536A410-32D2-4825-955D-4B523EB1628F}</c15:txfldGUID>
+                      <c15:txfldGUID>{EB7D6EFE-5C64-4846-88D1-0B6CF5BCCF05}</c15:txfldGUID>
                       <c15:f>calcs!$Y$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>08</c:v>
+                          <c:v>10</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5612,7 +5620,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>09</c:v>
+                      <c:v>11</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5628,12 +5636,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{16C255E4-A0E6-4716-A9CA-10EA2F9456D2}</c15:txfldGUID>
+                      <c15:txfldGUID>{45BB31F9-B6CE-4A30-ADD4-E3723F99D57F}</c15:txfldGUID>
                       <c15:f>calcs!$Z$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>09</c:v>
+                          <c:v>11</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5653,7 +5661,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>10</c:v>
+                      <c:v>12</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5669,12 +5677,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EFA5C9B9-F459-4553-8E10-7FD46DDA06D5}</c15:txfldGUID>
+                      <c15:txfldGUID>{D081A422-14F7-4F60-B900-58E82C11987A}</c15:txfldGUID>
                       <c15:f>calcs!$AA$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>10</c:v>
+                          <c:v>12</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5694,7 +5702,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>11</c:v>
+                      <c:v>13</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5710,12 +5718,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5DD59DC5-603B-4DA5-942E-69FD4D5EED45}</c15:txfldGUID>
+                      <c15:txfldGUID>{6C2FC7A5-7D23-4017-8831-F7186CAB830D}</c15:txfldGUID>
                       <c15:f>calcs!$AB$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>11</c:v>
+                          <c:v>13</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5735,7 +5743,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>12</c:v>
+                      <c:v>14</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5751,12 +5759,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29A1AD2A-EFD4-4AC8-B907-80B3F2D4BA9D}</c15:txfldGUID>
+                      <c15:txfldGUID>{48959C85-05EA-469A-965A-02F07846D840}</c15:txfldGUID>
                       <c15:f>calcs!$AC$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>12</c:v>
+                          <c:v>14</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5776,7 +5784,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>13</c:v>
+                      <c:v>15</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5792,12 +5800,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{76F3C3EF-9411-4FEC-BFD8-A13456D45E2C}</c15:txfldGUID>
+                      <c15:txfldGUID>{5F1C86FF-745E-4284-A015-C97850B0A049}</c15:txfldGUID>
                       <c15:f>calcs!$AD$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>13</c:v>
+                          <c:v>15</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5817,7 +5825,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>14</c:v>
+                      <c:v>16</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5833,12 +5841,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{180388CE-0A36-47B9-8982-5E668B572312}</c15:txfldGUID>
+                      <c15:txfldGUID>{C0DCCB2D-D13A-4773-BF6B-BD475C625EDF}</c15:txfldGUID>
                       <c15:f>calcs!$AE$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>14</c:v>
+                          <c:v>16</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5858,7 +5866,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>15</c:v>
+                      <c:v>17</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5874,12 +5882,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2EF1366F-BA2B-4E1D-832A-D0C1AC673B2B}</c15:txfldGUID>
+                      <c15:txfldGUID>{C30F9F71-8EB1-4324-B7CC-D798EB6B67AB}</c15:txfldGUID>
                       <c15:f>calcs!$AF$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>15</c:v>
+                          <c:v>17</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5899,7 +5907,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>16</c:v>
+                      <c:v>18</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5915,12 +5923,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{87C109A2-BC23-437B-A186-265A0F71B077}</c15:txfldGUID>
+                      <c15:txfldGUID>{F03CD120-2FB8-4AED-924E-F83B4F1FC8E6}</c15:txfldGUID>
                       <c15:f>calcs!$AG$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>16</c:v>
+                          <c:v>18</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -5940,7 +5948,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>17</c:v>
+                      <c:v>19</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -5956,12 +5964,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A6FA98A6-CA04-4917-8DE9-CFC3C959F30E}</c15:txfldGUID>
+                      <c15:txfldGUID>{523C7A7E-966C-4657-A06E-1C685D5F0CF3}</c15:txfldGUID>
                       <c15:f>calcs!$AH$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>17</c:v>
+                          <c:v>19</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6133,7 +6141,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>THU</c:v>
+                      <c:v>SAT</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6149,12 +6157,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8EE4827A-AF3A-41C3-AD86-2C2AF04CC3AD}</c15:txfldGUID>
+                      <c15:txfldGUID>{2080044A-C8F9-485F-8DD7-53D6089DB34C}</c15:txfldGUID>
                       <c15:f>calcs!$E$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>THU</c:v>
+                          <c:v>SAT</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6174,7 +6182,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>FRI</c:v>
+                      <c:v>SUN</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6190,12 +6198,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1F9DA0A6-2652-491A-B53B-4A8A146E98B2}</c15:txfldGUID>
+                      <c15:txfldGUID>{7BC971BE-3AB8-44EB-A7D5-8DBB611F5689}</c15:txfldGUID>
                       <c15:f>calcs!$F$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>FRI</c:v>
+                          <c:v>SUN</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6215,7 +6223,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SAT</c:v>
+                      <c:v>MON</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6231,12 +6239,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D933E98C-3F97-4C54-9BC8-B5284B9C4529}</c15:txfldGUID>
+                      <c15:txfldGUID>{A8E5482E-FDB9-40CA-B91B-42A16F1E9EC0}</c15:txfldGUID>
                       <c15:f>calcs!$G$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SAT</c:v>
+                          <c:v>MON</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6256,7 +6264,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SUN</c:v>
+                      <c:v>TUE</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6272,12 +6280,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0F5023CB-AF29-4672-84E6-EC9333C5C599}</c15:txfldGUID>
+                      <c15:txfldGUID>{6DF4D3F5-98A9-4A86-95F4-6EA98ADCBE8E}</c15:txfldGUID>
                       <c15:f>calcs!$H$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SUN</c:v>
+                          <c:v>TUE</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6297,7 +6305,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>MON</c:v>
+                      <c:v>WED</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6313,12 +6321,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0F1C7B0B-AD51-49C4-A45A-6B3243C4063F}</c15:txfldGUID>
+                      <c15:txfldGUID>{3DB093CD-7DBA-4A61-A984-E3D54C0D94A2}</c15:txfldGUID>
                       <c15:f>calcs!$I$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>MON</c:v>
+                          <c:v>WED</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6338,7 +6346,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>TUE</c:v>
+                      <c:v>THU</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6354,12 +6362,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6D9A130D-D3F2-4DBA-B447-736A38D7ADF1}</c15:txfldGUID>
+                      <c15:txfldGUID>{CD85990C-8397-4722-963D-0E31C0E04ED3}</c15:txfldGUID>
                       <c15:f>calcs!$J$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>TUE</c:v>
+                          <c:v>THU</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6379,7 +6387,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>WED</c:v>
+                      <c:v>FRI</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6395,12 +6403,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AE250DE5-0563-4AA1-8728-6DE5F2FAAA4C}</c15:txfldGUID>
+                      <c15:txfldGUID>{61661640-C530-43C9-8493-0DB06305ACB8}</c15:txfldGUID>
                       <c15:f>calcs!$K$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>WED</c:v>
+                          <c:v>FRI</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6420,7 +6428,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>THU</c:v>
+                      <c:v>SAT</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6436,12 +6444,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7686379B-8FFD-4480-ABFF-4E18E1E7F08B}</c15:txfldGUID>
+                      <c15:txfldGUID>{7C02F37C-C397-4B2A-AFBC-A20EAFEB0B2B}</c15:txfldGUID>
                       <c15:f>calcs!$L$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>THU</c:v>
+                          <c:v>SAT</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6461,7 +6469,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>FRI</c:v>
+                      <c:v>SUN</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6477,12 +6485,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{14918AE5-6548-4CC5-B913-7227ECFA9933}</c15:txfldGUID>
+                      <c15:txfldGUID>{80A9567F-F424-4CED-BD17-4A3D9A9774CD}</c15:txfldGUID>
                       <c15:f>calcs!$M$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>FRI</c:v>
+                          <c:v>SUN</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6502,7 +6510,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SAT</c:v>
+                      <c:v>MON</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6518,12 +6526,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{98AC67DF-451E-47B4-852C-B99D484D5C05}</c15:txfldGUID>
+                      <c15:txfldGUID>{1F027BF3-CB72-4696-9FCB-1A7A5A6285B0}</c15:txfldGUID>
                       <c15:f>calcs!$N$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SAT</c:v>
+                          <c:v>MON</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6543,7 +6551,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SUN</c:v>
+                      <c:v>TUE</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6559,12 +6567,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DF85A190-57F0-4ACD-B61E-CE2A8445F52F}</c15:txfldGUID>
+                      <c15:txfldGUID>{F6ABD8FA-D73B-4D69-AD10-CA5E44F82C2B}</c15:txfldGUID>
                       <c15:f>calcs!$O$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SUN</c:v>
+                          <c:v>TUE</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6584,7 +6592,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>MON</c:v>
+                      <c:v>WED</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6600,12 +6608,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D2A631EB-1960-44A7-9A1B-0C5802A869D8}</c15:txfldGUID>
+                      <c15:txfldGUID>{D0280DBA-7E42-47CB-B4B0-DD4BF8C61B61}</c15:txfldGUID>
                       <c15:f>calcs!$P$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>MON</c:v>
+                          <c:v>WED</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6625,7 +6633,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>TUE</c:v>
+                      <c:v>THU</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6641,12 +6649,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B13BBFCC-45E2-4493-AFB4-1092C4154339}</c15:txfldGUID>
+                      <c15:txfldGUID>{07DD534C-0BD6-42D6-A848-3819DA827F64}</c15:txfldGUID>
                       <c15:f>calcs!$Q$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>TUE</c:v>
+                          <c:v>THU</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6666,7 +6674,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>WED</c:v>
+                      <c:v>FRI</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6682,12 +6690,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{66DB7416-80F3-4A1B-8BF8-A966B719E2E6}</c15:txfldGUID>
+                      <c15:txfldGUID>{F487F989-3E38-4ED7-B0E4-977E99511E54}</c15:txfldGUID>
                       <c15:f>calcs!$R$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>WED</c:v>
+                          <c:v>FRI</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6707,7 +6715,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>THU</c:v>
+                      <c:v>SAT</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6723,12 +6731,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C73B9183-2F76-4C16-8429-649F3D5A24B9}</c15:txfldGUID>
+                      <c15:txfldGUID>{D53DC6FE-D924-4224-B1B6-FCB4E14A55C9}</c15:txfldGUID>
                       <c15:f>calcs!$S$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>THU</c:v>
+                          <c:v>SAT</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6748,7 +6756,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>FRI</c:v>
+                      <c:v>SUN</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6764,12 +6772,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{75516503-B3F6-45A3-AACD-930CC4DD5C84}</c15:txfldGUID>
+                      <c15:txfldGUID>{18FACCC1-B64D-4E21-BCC8-9FBC4299BD8D}</c15:txfldGUID>
                       <c15:f>calcs!$T$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>FRI</c:v>
+                          <c:v>SUN</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6789,7 +6797,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SAT</c:v>
+                      <c:v>MON</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6805,12 +6813,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{06D96B84-AB4F-4E51-A2E6-55E02BBB888A}</c15:txfldGUID>
+                      <c15:txfldGUID>{F42D9FC8-4C99-457D-9308-57E66DB004CB}</c15:txfldGUID>
                       <c15:f>calcs!$U$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SAT</c:v>
+                          <c:v>MON</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6830,7 +6838,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SUN</c:v>
+                      <c:v>TUE</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6846,12 +6854,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{26E7664B-E150-404A-B415-FD113202B66F}</c15:txfldGUID>
+                      <c15:txfldGUID>{A3EDEED3-51CE-466B-9397-50120FEF38AB}</c15:txfldGUID>
                       <c15:f>calcs!$V$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SUN</c:v>
+                          <c:v>TUE</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6871,7 +6879,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>MON</c:v>
+                      <c:v>WED</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6887,12 +6895,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7CB49AC2-7572-4112-88BD-11623E2FC5BC}</c15:txfldGUID>
+                      <c15:txfldGUID>{D68A2B9E-D6F3-4F3A-AC8C-D733246258E4}</c15:txfldGUID>
                       <c15:f>calcs!$W$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>MON</c:v>
+                          <c:v>WED</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6912,7 +6920,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>TUE</c:v>
+                      <c:v>THU</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6928,12 +6936,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{55DFD423-5035-4E94-9E9E-0BA3C9ABCCA3}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE5A4382-8E6E-4F9E-9D29-31CF1244871C}</c15:txfldGUID>
                       <c15:f>calcs!$X$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>TUE</c:v>
+                          <c:v>THU</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6953,7 +6961,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>WED</c:v>
+                      <c:v>FRI</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -6969,12 +6977,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EAAE95D8-1AF5-49D2-AA8D-E4F58D9829D7}</c15:txfldGUID>
+                      <c15:txfldGUID>{4B8B84B2-38DE-4023-A32A-A575F5B3DB08}</c15:txfldGUID>
                       <c15:f>calcs!$Y$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>WED</c:v>
+                          <c:v>FRI</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -6994,7 +7002,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>THU</c:v>
+                      <c:v>SAT</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7010,12 +7018,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8500CD07-CECB-404C-B2AB-AB768CF2C617}</c15:txfldGUID>
+                      <c15:txfldGUID>{D6831FAB-4A83-48DF-BA6B-9E16165C8337}</c15:txfldGUID>
                       <c15:f>calcs!$Z$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>THU</c:v>
+                          <c:v>SAT</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7035,7 +7043,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>FRI</c:v>
+                      <c:v>SUN</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7051,12 +7059,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1461161D-C326-4B14-ACA1-06135E3FE913}</c15:txfldGUID>
+                      <c15:txfldGUID>{EA0750C2-9254-4C38-B520-975760EA621F}</c15:txfldGUID>
                       <c15:f>calcs!$AA$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>FRI</c:v>
+                          <c:v>SUN</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7076,7 +7084,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SAT</c:v>
+                      <c:v>MON</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7092,12 +7100,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D0D7E1AB-EBEE-462F-84C5-88332ABCC4DB}</c15:txfldGUID>
+                      <c15:txfldGUID>{8E742D94-A34C-428E-BAD5-58AF28F68A7F}</c15:txfldGUID>
                       <c15:f>calcs!$AB$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SAT</c:v>
+                          <c:v>MON</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7117,7 +7125,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>SUN</c:v>
+                      <c:v>TUE</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7133,12 +7141,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9DB5018C-2EA2-4DCF-B8A9-4BB24F3A8740}</c15:txfldGUID>
+                      <c15:txfldGUID>{B78C8985-2DDA-441C-BA47-254C193CD36C}</c15:txfldGUID>
                       <c15:f>calcs!$AC$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>SUN</c:v>
+                          <c:v>TUE</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7158,7 +7166,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>MON</c:v>
+                      <c:v>WED</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7174,12 +7182,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8D4721CC-A40A-4507-AB2E-781FFC3C8374}</c15:txfldGUID>
+                      <c15:txfldGUID>{C400BA6C-8753-4EC2-AAFF-E20CEE1AEBFC}</c15:txfldGUID>
                       <c15:f>calcs!$AD$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>MON</c:v>
+                          <c:v>WED</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7199,7 +7207,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>TUE</c:v>
+                      <c:v>THU</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7215,12 +7223,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CC62A564-315C-4324-8A08-A4C731C6F8A0}</c15:txfldGUID>
+                      <c15:txfldGUID>{55689802-16DD-46F1-9A51-8A11F5696DB7}</c15:txfldGUID>
                       <c15:f>calcs!$AE$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>TUE</c:v>
+                          <c:v>THU</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7240,7 +7248,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>WED</c:v>
+                      <c:v>FRI</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7256,12 +7264,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BBA71740-4596-42F2-AD3F-B697BE3552C9}</c15:txfldGUID>
+                      <c15:txfldGUID>{70A33ADF-FEB8-46F4-A5BC-AB5EE3CBFF11}</c15:txfldGUID>
                       <c15:f>calcs!$AF$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>WED</c:v>
+                          <c:v>FRI</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7281,7 +7289,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>THU</c:v>
+                      <c:v>SAT</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7297,12 +7305,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{18350D16-CC4E-4E7B-A29C-41EC9AE52F88}</c15:txfldGUID>
+                      <c15:txfldGUID>{5D30A616-2A17-4160-A5E0-001DAEC3DDEF}</c15:txfldGUID>
                       <c15:f>calcs!$AG$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>THU</c:v>
+                          <c:v>SAT</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7322,7 +7330,7 @@
                   <c:strCache>
                     <c:ptCount val="1"/>
                     <c:pt idx="0">
-                      <c:v>FRI</c:v>
+                      <c:v>SUN</c:v>
                     </c:pt>
                   </c:strCache>
                 </c:strRef>
@@ -7338,12 +7346,12 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{90DF15AA-2AA5-4B1F-9812-E2E81CDBD708}</c15:txfldGUID>
+                      <c15:txfldGUID>{A050FBCF-214E-4B1D-AB7C-6EF6E1596DF6}</c15:txfldGUID>
                       <c15:f>calcs!$AH$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>FRI</c:v>
+                          <c:v>SUN</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -7558,10 +7566,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -7691,10 +7699,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>13</c:v>
@@ -7917,8 +7925,8 @@
         <a:xfrm>
           <a:off x="337028" y="4046499"/>
           <a:ext cx="9246078" cy="228436"/>
-          <a:chOff x="306828" y="4108026"/>
-          <a:chExt cx="8729080" cy="223568"/>
+          <a:chOff x="306828" y="4108028"/>
+          <a:chExt cx="8729080" cy="223566"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -7992,7 +8000,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="306828" y="4108026"/>
+                <a:off x="306828" y="4108028"/>
                 <a:ext cx="8729080" cy="163196"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -8278,8 +8286,8 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8321,7 +8329,7 @@
       </c>
       <c r="D3" s="8">
         <f ca="1">TODAY()</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8338,10 +8346,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>16</v>
@@ -8371,7 +8379,7 @@
         <v>-9</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D6" s="12">
         <v>44972</v>
@@ -8379,10 +8387,12 @@
       <c r="E6" s="12">
         <v>44975</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="G6" s="12"/>
       <c r="H6" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8402,16 +8412,16 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <f>ROW(B8)-calcs!$D$5</f>
         <v>-7</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12">
         <v>44976</v>
@@ -8419,59 +8429,60 @@
       <c r="E8" s="12">
         <v>44978</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <f>ROW(B9)-calcs!$D$5</f>
-        <v>-6</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D9" s="12">
-        <v>44976</v>
+        <v>44978</v>
       </c>
       <c r="E9" s="12">
         <v>44978</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="H9" s="11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <f>ROW(B10)-calcs!$D$5</f>
-        <v>-5</v>
-      </c>
       <c r="C10" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D10" s="12">
         <v>44976</v>
       </c>
       <c r="E10" s="12">
+        <f>Activities[[#This Row],[START]]+2</f>
         <v>44978</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <f>ROW(B11)-calcs!$D$5</f>
-        <v>-4</v>
-      </c>
       <c r="C11" s="11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D11" s="12">
         <v>44978</v>
@@ -8479,27 +8490,18 @@
       <c r="E11" s="12">
         <v>44979</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="F11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <f>ROW(B12)-calcs!$D$5</f>
-        <v>-3</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="12">
-        <v>44976</v>
-      </c>
-      <c r="E12" s="12">
-        <f>Activities[[#This Row],[START]]+2</f>
-        <v>44978</v>
-      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="11"/>
@@ -8509,37 +8511,21 @@
         <f>ROW(B13)-calcs!$D$5</f>
         <v>-2</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="12">
-        <v>44976</v>
-      </c>
-      <c r="E13" s="12">
-        <f>Activities[[#This Row],[START]]+2</f>
-        <v>44978</v>
-      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>ROW(B14)-calcs!$D$5</f>
         <v>-1</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="12">
-        <v>44976</v>
-      </c>
-      <c r="E14" s="12">
-        <f>Activities[[#This Row],[START]]+2</f>
-        <v>44978</v>
-      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="11"/>
@@ -8671,7 +8657,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">TODAY()</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -8713,7 +8699,7 @@
       </c>
       <c r="D9">
         <f ca="1">SUMPRODUCT( ((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)) )</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" t="e">
         <f>NA()</f>
@@ -8732,7 +8718,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11">
         <f ca="1">D10-MIN(D10,D9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="e">
         <f>NA()</f>
@@ -8765,9 +8751,9 @@
         <f t="array" aca="1" ref="E15" ca="1">INDEX(Activities[Id],MATCH(1, ((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>-9</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="e">
         <f t="shared" ref="F15:F23" ca="1" si="0">OFFSET(E15,-$D$11,)</f>
-        <v>-9</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -8776,9 +8762,9 @@
         <f t="array" aca="1" ref="E16" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E15)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>-8</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
@@ -8787,69 +8773,69 @@
         <f t="array" aca="1" ref="E17" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E16)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>-7</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E18">
         <f t="array" aca="1" ref="E18" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E17)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="E19">
+      <c r="E19" t="e">
         <f t="array" aca="1" ref="E19" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E18)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-5</v>
+        <v>#N/A</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="E20">
+      <c r="E20" t="e">
         <f t="array" aca="1" ref="E20" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E19)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-4</v>
+        <v>#N/A</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="E21">
+      <c r="E21" t="e">
         <f t="array" aca="1" ref="E21" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E20)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-3</v>
+        <v>#N/A</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="E22">
+      <c r="E22" t="e">
         <f t="array" aca="1" ref="E22" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E21)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-2</v>
-      </c>
-      <c r="F22">
+        <v>#N/A</v>
+      </c>
+      <c r="F22" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="E23">
+      <c r="E23" t="e">
         <f t="array" aca="1" ref="E23" ca="1">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E22)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
-        <v>-1</v>
-      </c>
-      <c r="F23">
+        <v>#N/A</v>
+      </c>
+      <c r="F23" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
@@ -8858,7 +8844,7 @@
       </c>
       <c r="D25" s="1">
         <f ca="1">StartDate+WindowOffset</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
@@ -8875,7 +8861,7 @@
       </c>
       <c r="D28" s="2">
         <f ca="1">'Project Timeline'!D3</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
@@ -8901,127 +8887,127 @@
       </c>
       <c r="E31" s="1">
         <f ca="1">StartDateWindow</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ref="F31:AI31" ca="1" si="1">E31+1</f>
-        <v>44974</v>
+        <v>44976</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44975</v>
+        <v>44977</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44976</v>
+        <v>44978</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44977</v>
+        <v>44979</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44978</v>
+        <v>44980</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44979</v>
+        <v>44981</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44980</v>
+        <v>44982</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44981</v>
+        <v>44983</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44982</v>
+        <v>44984</v>
       </c>
       <c r="O31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44983</v>
+        <v>44985</v>
       </c>
       <c r="P31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44984</v>
+        <v>44986</v>
       </c>
       <c r="Q31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44985</v>
+        <v>44987</v>
       </c>
       <c r="R31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44986</v>
+        <v>44988</v>
       </c>
       <c r="S31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44987</v>
+        <v>44989</v>
       </c>
       <c r="T31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="U31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44989</v>
+        <v>44991</v>
       </c>
       <c r="V31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44990</v>
+        <v>44992</v>
       </c>
       <c r="W31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="X31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="Y31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="Z31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44994</v>
+        <v>44996</v>
       </c>
       <c r="AA31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44995</v>
+        <v>44997</v>
       </c>
       <c r="AB31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44996</v>
+        <v>44998</v>
       </c>
       <c r="AC31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44997</v>
+        <v>44999</v>
       </c>
       <c r="AD31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="AE31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44999</v>
+        <v>45001</v>
       </c>
       <c r="AF31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45000</v>
+        <v>45002</v>
       </c>
       <c r="AG31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="AH31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45002</v>
+        <v>45004</v>
       </c>
       <c r="AI31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45003</v>
+        <v>45005</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
@@ -9031,25 +9017,25 @@
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="e">
         <f t="shared" ref="C32:C40" ca="1" si="2">F15</f>
-        <v>-9</v>
-      </c>
-      <c r="D32" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D32" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C32,Activities[Id],0))</f>
-        <v>Preparation</v>
-      </c>
-      <c r="E32">
-        <f ca="1">GridCalc</f>
-        <v>11.3</v>
-      </c>
-      <c r="F32">
-        <f ca="1">GridCalc</f>
-        <v>11.3</v>
-      </c>
-      <c r="G32">
-        <f ca="1">GridCalc</f>
-        <v>11.3</v>
+        <v>#N/A</v>
+      </c>
+      <c r="E32" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F32" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="H32" t="e">
         <f ca="1">GridCalc</f>
@@ -9172,13 +9158,13 @@
       <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>-8</v>
-      </c>
-      <c r="D33" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D33" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C33,Activities[Id],0))</f>
-        <v>First Meeting</v>
+        <v>#N/A</v>
       </c>
       <c r="E33" t="e">
         <f ca="1">GridCalc</f>
@@ -9188,9 +9174,9 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="G33">
-        <f ca="1">GridCalc</f>
-        <v>10.3</v>
+      <c r="G33" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="H33" t="e">
         <f ca="1">GridCalc</f>
@@ -9313,13 +9299,13 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="D34" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D34" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C34,Activities[Id],0))</f>
-        <v>Proposal -1</v>
+        <v>#N/A</v>
       </c>
       <c r="E34" t="e">
         <f ca="1">GridCalc</f>
@@ -9333,17 +9319,17 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="H34">
-        <f ca="1">GridCalc</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="I34">
-        <f ca="1">GridCalc</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J34">
-        <f ca="1">GridCalc</f>
-        <v>9.3000000000000007</v>
+      <c r="H34" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I34" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J34" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K34" t="e">
         <f ca="1">GridCalc</f>
@@ -9456,15 +9442,15 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="2"/>
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="D35" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C35,Activities[Id],0))</f>
-        <v>Proposal -2</v>
-      </c>
-      <c r="E35" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+        <v>Brainstorming</v>
+      </c>
+      <c r="E35">
+        <f ca="1">GridCalc</f>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F35" t="e">
         <f ca="1">GridCalc</f>
@@ -9474,17 +9460,17 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="H35">
-        <f ca="1">GridCalc</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I35">
-        <f ca="1">GridCalc</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J35">
-        <f ca="1">GridCalc</f>
-        <v>8.3000000000000007</v>
+      <c r="H35" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I35" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J35" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K35" t="e">
         <f ca="1">GridCalc</f>
@@ -9597,15 +9583,15 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="2"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="D36" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C36,Activities[Id],0))</f>
-        <v>Proposal -3</v>
-      </c>
-      <c r="E36" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+        <v>First Meeting</v>
+      </c>
+      <c r="E36">
+        <f ca="1">GridCalc</f>
+        <v>7.3000000000000007</v>
       </c>
       <c r="F36" t="e">
         <f ca="1">GridCalc</f>
@@ -9615,17 +9601,17 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="H36">
-        <f ca="1">GridCalc</f>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="I36">
-        <f ca="1">GridCalc</f>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J36">
-        <f ca="1">GridCalc</f>
-        <v>7.3000000000000007</v>
+      <c r="H36" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I36" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J36" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K36" t="e">
         <f ca="1">GridCalc</f>
@@ -9738,39 +9724,39 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="2"/>
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="D37" t="str">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C37,Activities[Id],0))</f>
-        <v>README.md</v>
+        <v xml:space="preserve">Proposal </v>
       </c>
       <c r="E37" t="e">
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="F37" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G37" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H37" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+      <c r="F37">
+        <f ca="1">GridCalc</f>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="G37">
+        <f ca="1">GridCalc</f>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="H37">
+        <f ca="1">GridCalc</f>
+        <v>6.3000000000000007</v>
       </c>
       <c r="I37" t="e">
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="J37">
-        <f ca="1">GridCalc</f>
-        <v>6.3000000000000007</v>
-      </c>
-      <c r="K37">
-        <f ca="1">GridCalc</f>
-        <v>6.3000000000000007</v>
+      <c r="J37" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K37" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="L37" t="e">
         <f ca="1">GridCalc</f>
@@ -9869,7 +9855,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>5.3000000000000007</v>
@@ -9879,36 +9865,35 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
-      </c>
-      <c r="D38" t="str">
+        <v>0</v>
+      </c>
+      <c r="D38" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C38,Activities[Id],0))</f>
-        <v>Team work contract
-team-contract.md</v>
+        <v>#N/A</v>
       </c>
       <c r="E38" t="e">
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="F38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G38" t="e">
-        <f ca="1">GridCalc</f>
-        <v>#N/A</v>
+      <c r="F38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="G38">
+        <f ca="1">GridCalc</f>
+        <v>5.3000000000000007</v>
       </c>
       <c r="H38">
         <f ca="1">GridCalc</f>
+        <v>1.7666666666666668</v>
+      </c>
+      <c r="I38">
+        <f ca="1">GridCalc</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="I38">
-        <f ca="1">GridCalc</f>
-        <v>5.3000000000000007</v>
-      </c>
-      <c r="J38">
-        <f ca="1">GridCalc</f>
-        <v>5.3000000000000007</v>
+      <c r="J38" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K38" t="e">
         <f ca="1">GridCalc</f>
@@ -10011,7 +9996,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>4.3000000000000007</v>
@@ -10019,13 +10004,13 @@
       <c r="B39">
         <v>8</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
-      </c>
-      <c r="D39" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D39" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C39,Activities[Id],0))</f>
-        <v>CODE_OF_CONDUCT.md</v>
+        <v>#N/A</v>
       </c>
       <c r="E39" t="e">
         <f ca="1">GridCalc</f>
@@ -10039,17 +10024,17 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="H39">
-        <f ca="1">GridCalc</f>
-        <v>4.3000000000000007</v>
-      </c>
-      <c r="I39">
-        <f ca="1">GridCalc</f>
-        <v>4.3000000000000007</v>
-      </c>
-      <c r="J39">
-        <f ca="1">GridCalc</f>
-        <v>4.3000000000000007</v>
+      <c r="H39" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I39" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J39" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K39" t="e">
         <f ca="1">GridCalc</f>
@@ -10152,7 +10137,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>3.3000000000000007</v>
@@ -10160,13 +10145,13 @@
       <c r="B40">
         <v>9</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="D40" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D40" t="e">
         <f ca="1">INDEX(Activities[ACTIVITY],MATCH($C40,Activities[Id],0))</f>
-        <v>CONTRIBUTING.md</v>
+        <v>#N/A</v>
       </c>
       <c r="E40" t="e">
         <f ca="1">GridCalc</f>
@@ -10180,17 +10165,17 @@
         <f ca="1">GridCalc</f>
         <v>#N/A</v>
       </c>
-      <c r="H40">
-        <f ca="1">GridCalc</f>
-        <v>3.3000000000000007</v>
-      </c>
-      <c r="I40">
-        <f ca="1">GridCalc</f>
-        <v>3.3000000000000007</v>
-      </c>
-      <c r="J40">
-        <f ca="1">GridCalc</f>
-        <v>3.3000000000000007</v>
+      <c r="H40" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I40" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J40" t="e">
+        <f ca="1">GridCalc</f>
+        <v>#N/A</v>
       </c>
       <c r="K40" t="e">
         <f ca="1">GridCalc</f>
@@ -10296,133 +10281,133 @@
     <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E43" s="1">
         <f ca="1">E31</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ref="F43:AH43" ca="1" si="4">F31</f>
-        <v>44974</v>
+        <v>44976</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44975</v>
+        <v>44977</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44976</v>
+        <v>44978</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44977</v>
+        <v>44979</v>
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44978</v>
+        <v>44980</v>
       </c>
       <c r="K43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44979</v>
+        <v>44981</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44980</v>
+        <v>44982</v>
       </c>
       <c r="M43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44981</v>
+        <v>44983</v>
       </c>
       <c r="N43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44982</v>
+        <v>44984</v>
       </c>
       <c r="O43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44983</v>
+        <v>44985</v>
       </c>
       <c r="P43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44984</v>
+        <v>44986</v>
       </c>
       <c r="Q43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44985</v>
+        <v>44987</v>
       </c>
       <c r="R43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44986</v>
+        <v>44988</v>
       </c>
       <c r="S43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44987</v>
+        <v>44989</v>
       </c>
       <c r="T43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="U43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44989</v>
+        <v>44991</v>
       </c>
       <c r="V43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44990</v>
+        <v>44992</v>
       </c>
       <c r="W43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="X43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="Y43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="Z43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44994</v>
+        <v>44996</v>
       </c>
       <c r="AA43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44995</v>
+        <v>44997</v>
       </c>
       <c r="AB43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44996</v>
+        <v>44998</v>
       </c>
       <c r="AC43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44997</v>
+        <v>44999</v>
       </c>
       <c r="AD43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="AE43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44999</v>
+        <v>45001</v>
       </c>
       <c r="AF43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>45000</v>
+        <v>45002</v>
       </c>
       <c r="AG43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="AH43" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>45002</v>
+        <v>45004</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="C44">
+      <c r="C44" t="e">
         <f ca="1">C32</f>
-        <v>-9</v>
-      </c>
-      <c r="D44" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D44" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C44,Activities[Id],0)))</f>
-        <v>PREPARATION</v>
+        <v>#N/A</v>
       </c>
       <c r="E44" t="e">
         <f t="shared" ref="E44:AH44" ca="1" si="5">IF(ISERROR(F32),E32,NA())</f>
@@ -10432,9 +10417,9 @@
         <f t="shared" ca="1" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G44">
+      <c r="G44" t="e">
         <f t="shared" ca="1" si="5"/>
-        <v>11.3</v>
+        <v>#N/A</v>
       </c>
       <c r="H44" t="e">
         <f t="shared" ca="1" si="5"/>
@@ -10546,13 +10531,13 @@
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="C45">
+      <c r="C45" t="e">
         <f t="shared" ref="C45:C52" ca="1" si="6">C33</f>
-        <v>-8</v>
-      </c>
-      <c r="D45" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D45" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C45,Activities[Id],0)))</f>
-        <v>FIRST MEETING</v>
+        <v>#N/A</v>
       </c>
       <c r="E45" t="e">
         <f t="shared" ref="E45:AH45" ca="1" si="7">IF(ISERROR(F33),E33,NA())</f>
@@ -10562,9 +10547,9 @@
         <f t="shared" ca="1" si="7"/>
         <v>#N/A</v>
       </c>
-      <c r="G45">
+      <c r="G45" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>10.3</v>
+        <v>#N/A</v>
       </c>
       <c r="H45" t="e">
         <f t="shared" ca="1" si="7"/>
@@ -10676,13 +10661,13 @@
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="C46">
+      <c r="C46" t="e">
         <f t="shared" ca="1" si="6"/>
-        <v>-7</v>
-      </c>
-      <c r="D46" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D46" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C46,Activities[Id],0)))</f>
-        <v>PROPOSAL -1</v>
+        <v>#N/A</v>
       </c>
       <c r="E46" t="e">
         <f t="shared" ref="E46:AH46" ca="1" si="8">IF(ISERROR(F34),E34,NA())</f>
@@ -10704,9 +10689,9 @@
         <f t="shared" ca="1" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="J46">
+      <c r="J46" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>9.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="K46" t="e">
         <f t="shared" ca="1" si="8"/>
@@ -10808,15 +10793,15 @@
     <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C47">
         <f t="shared" ca="1" si="6"/>
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="D47" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C47,Activities[Id],0)))</f>
-        <v>PROPOSAL -2</v>
-      </c>
-      <c r="E47" t="e">
+        <v>BRAINSTORMING</v>
+      </c>
+      <c r="E47">
         <f t="shared" ref="E47:AH47" ca="1" si="9">IF(ISERROR(F35),E35,NA())</f>
-        <v>#N/A</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F47" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -10834,9 +10819,9 @@
         <f t="shared" ca="1" si="9"/>
         <v>#N/A</v>
       </c>
-      <c r="J47">
+      <c r="J47" t="e">
         <f t="shared" ca="1" si="9"/>
-        <v>8.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="K47" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -10938,15 +10923,15 @@
     <row r="48" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C48">
         <f t="shared" ca="1" si="6"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="D48" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C48,Activities[Id],0)))</f>
-        <v>PROPOSAL -3</v>
-      </c>
-      <c r="E48" t="e">
+        <v>FIRST MEETING</v>
+      </c>
+      <c r="E48">
         <f t="shared" ref="E48:AH48" ca="1" si="10">IF(ISERROR(F36),E36,NA())</f>
-        <v>#N/A</v>
+        <v>7.3000000000000007</v>
       </c>
       <c r="F48" t="e">
         <f t="shared" ca="1" si="10"/>
@@ -10964,9 +10949,9 @@
         <f t="shared" ca="1" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="J48">
+      <c r="J48" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v>7.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="K48" t="e">
         <f t="shared" ca="1" si="10"/>
@@ -11068,11 +11053,11 @@
     <row r="49" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C49">
         <f t="shared" ca="1" si="6"/>
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="D49" t="str">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C49,Activities[Id],0)))</f>
-        <v>README.MD</v>
+        <v xml:space="preserve">PROPOSAL </v>
       </c>
       <c r="E49" t="e">
         <f t="shared" ref="E49:AH49" ca="1" si="11">IF(ISERROR(F37),E37,NA())</f>
@@ -11086,9 +11071,9 @@
         <f t="shared" ca="1" si="11"/>
         <v>#N/A</v>
       </c>
-      <c r="H49" t="e">
+      <c r="H49">
         <f t="shared" ca="1" si="11"/>
-        <v>#N/A</v>
+        <v>6.3000000000000007</v>
       </c>
       <c r="I49" t="e">
         <f t="shared" ca="1" si="11"/>
@@ -11098,9 +11083,9 @@
         <f t="shared" ca="1" si="11"/>
         <v>#N/A</v>
       </c>
-      <c r="K49">
+      <c r="K49" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>6.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="L49" t="e">
         <f t="shared" ca="1" si="11"/>
@@ -11195,15 +11180,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="3:34" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C50">
         <f t="shared" ca="1" si="6"/>
-        <v>-3</v>
-      </c>
-      <c r="D50" t="str">
+        <v>0</v>
+      </c>
+      <c r="D50" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C50,Activities[Id],0)))</f>
-        <v>TEAM WORK CONTRACT
-TEAM-CONTRACT.MD</v>
+        <v>#N/A</v>
       </c>
       <c r="E50" t="e">
         <f t="shared" ref="E50:AH50" ca="1" si="12">IF(ISERROR(F38),E38,NA())</f>
@@ -11221,14 +11205,14 @@
         <f t="shared" ca="1" si="12"/>
         <v>#N/A</v>
       </c>
-      <c r="I50" t="e">
-        <f t="shared" ca="1" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J50">
+      <c r="I50">
         <f t="shared" ca="1" si="12"/>
         <v>5.3000000000000007</v>
       </c>
+      <c r="J50" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#N/A</v>
+      </c>
       <c r="K50" t="e">
         <f t="shared" ca="1" si="12"/>
         <v>#N/A</v>
@@ -11326,14 +11310,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="3:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C51">
+    <row r="51" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C51" t="e">
         <f t="shared" ca="1" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="D51" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D51" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C51,Activities[Id],0)))</f>
-        <v>CODE_OF_CONDUCT.MD</v>
+        <v>#N/A</v>
       </c>
       <c r="E51" t="e">
         <f t="shared" ref="E51:AH51" ca="1" si="13">IF(ISERROR(F39),E39,NA())</f>
@@ -11355,9 +11339,9 @@
         <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
-      <c r="J51">
+      <c r="J51" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>4.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="K51" t="e">
         <f t="shared" ca="1" si="13"/>
@@ -11456,14 +11440,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="3:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C52">
+    <row r="52" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C52" t="e">
         <f t="shared" ca="1" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="D52" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D52" t="e">
         <f ca="1">UPPER(INDEX(Activities[ACTIVITY],MATCH($C52,Activities[Id],0)))</f>
-        <v>CONTRIBUTING.MD</v>
+        <v>#N/A</v>
       </c>
       <c r="E52" t="e">
         <f t="shared" ref="E52:AH52" ca="1" si="14">IF(ISERROR(F40),E40,NA())</f>
@@ -11485,9 +11469,9 @@
         <f t="shared" ca="1" si="14"/>
         <v>#N/A</v>
       </c>
-      <c r="J52">
+      <c r="J52" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>3.3000000000000007</v>
+        <v>#N/A</v>
       </c>
       <c r="K52" t="e">
         <f t="shared" ca="1" si="14"/>
@@ -11589,123 +11573,123 @@
     <row r="55" spans="3:34" x14ac:dyDescent="0.3">
       <c r="E55" s="1">
         <f ca="1">E31</f>
-        <v>44973</v>
+        <v>44975</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" ref="F55:AH55" ca="1" si="15">F31</f>
-        <v>44974</v>
+        <v>44976</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44975</v>
+        <v>44977</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44976</v>
+        <v>44978</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44977</v>
+        <v>44979</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44978</v>
+        <v>44980</v>
       </c>
       <c r="K55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44979</v>
+        <v>44981</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44980</v>
+        <v>44982</v>
       </c>
       <c r="M55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44981</v>
+        <v>44983</v>
       </c>
       <c r="N55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44982</v>
+        <v>44984</v>
       </c>
       <c r="O55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44983</v>
+        <v>44985</v>
       </c>
       <c r="P55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44984</v>
+        <v>44986</v>
       </c>
       <c r="Q55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44985</v>
+        <v>44987</v>
       </c>
       <c r="R55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44986</v>
+        <v>44988</v>
       </c>
       <c r="S55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44987</v>
+        <v>44989</v>
       </c>
       <c r="T55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="U55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44989</v>
+        <v>44991</v>
       </c>
       <c r="V55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44990</v>
+        <v>44992</v>
       </c>
       <c r="W55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="X55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="Y55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="Z55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44994</v>
+        <v>44996</v>
       </c>
       <c r="AA55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44995</v>
+        <v>44997</v>
       </c>
       <c r="AB55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44996</v>
+        <v>44998</v>
       </c>
       <c r="AC55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44997</v>
+        <v>44999</v>
       </c>
       <c r="AD55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="AE55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>44999</v>
+        <v>45001</v>
       </c>
       <c r="AF55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>45000</v>
+        <v>45002</v>
       </c>
       <c r="AG55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="AH55" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>45002</v>
+        <v>45004</v>
       </c>
     </row>
     <row r="56" spans="3:34" x14ac:dyDescent="0.3">
@@ -11882,13 +11866,13 @@
         <f t="shared" ca="1" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P58">
+      <c r="P58" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q58">
+        <v>#N/A</v>
+      </c>
+      <c r="Q58" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="R58" t="e">
         <f t="shared" ca="1" si="17"/>
@@ -12008,13 +11992,13 @@
         <f t="shared" ca="1" si="18"/>
         <v>13</v>
       </c>
-      <c r="P59">
+      <c r="P59" t="e">
         <f t="shared" ca="1" si="18"/>
-        <v>13</v>
-      </c>
-      <c r="Q59">
+        <v>#N/A</v>
+      </c>
+      <c r="Q59" t="e">
         <f t="shared" ca="1" si="18"/>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
       <c r="R59" t="e">
         <f t="shared" ca="1" si="18"/>
@@ -12137,13 +12121,13 @@
         <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
-      <c r="P61" t="e">
+      <c r="P61">
         <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q61" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="Q61">
         <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="R61">
         <f t="shared" ca="1" si="19"/>
@@ -12263,13 +12247,13 @@
         <f t="shared" ca="1" si="20"/>
         <v>#N/A</v>
       </c>
-      <c r="P62" t="e">
+      <c r="P62">
         <f t="shared" ca="1" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q62" t="e">
+        <v>13</v>
+      </c>
+      <c r="Q62">
         <f t="shared" ca="1" si="20"/>
-        <v>#N/A</v>
+        <v>13</v>
       </c>
       <c r="R62">
         <f t="shared" ca="1" si="20"/>
@@ -12522,17 +12506,17 @@
         <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
-      <c r="Q66" t="e">
+      <c r="Q66">
         <f t="shared" ca="1" si="21"/>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="R66" t="e">
         <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
-      <c r="S66">
+      <c r="S66" t="e">
         <f t="shared" ca="1" si="21"/>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="T66" t="e">
         <f t="shared" ca="1" si="21"/>
@@ -12722,123 +12706,123 @@
       </c>
       <c r="E70" t="str">
         <f ca="1">LEFT(UPPER(TEXT(E55,"ddd")),$D70)</f>
-        <v>THU</v>
+        <v>SAT</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" ref="F70:AH70" ca="1" si="23">LEFT(UPPER(TEXT(F55,"ddd")),$D70)</f>
-        <v>FRI</v>
+        <v>SUN</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SAT</v>
+        <v>MON</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SUN</v>
+        <v>TUE</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>MON</v>
+        <v>WED</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>TUE</v>
+        <v>THU</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>WED</v>
+        <v>FRI</v>
       </c>
       <c r="L70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>THU</v>
+        <v>SAT</v>
       </c>
       <c r="M70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>FRI</v>
+        <v>SUN</v>
       </c>
       <c r="N70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SAT</v>
+        <v>MON</v>
       </c>
       <c r="O70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SUN</v>
+        <v>TUE</v>
       </c>
       <c r="P70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>MON</v>
+        <v>WED</v>
       </c>
       <c r="Q70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>TUE</v>
+        <v>THU</v>
       </c>
       <c r="R70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>WED</v>
+        <v>FRI</v>
       </c>
       <c r="S70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>THU</v>
+        <v>SAT</v>
       </c>
       <c r="T70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>FRI</v>
+        <v>SUN</v>
       </c>
       <c r="U70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SAT</v>
+        <v>MON</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SUN</v>
+        <v>TUE</v>
       </c>
       <c r="W70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>MON</v>
+        <v>WED</v>
       </c>
       <c r="X70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>TUE</v>
+        <v>THU</v>
       </c>
       <c r="Y70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>WED</v>
+        <v>FRI</v>
       </c>
       <c r="Z70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>THU</v>
+        <v>SAT</v>
       </c>
       <c r="AA70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>FRI</v>
+        <v>SUN</v>
       </c>
       <c r="AB70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SAT</v>
+        <v>MON</v>
       </c>
       <c r="AC70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>SUN</v>
+        <v>TUE</v>
       </c>
       <c r="AD70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>MON</v>
+        <v>WED</v>
       </c>
       <c r="AE70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>TUE</v>
+        <v>THU</v>
       </c>
       <c r="AF70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>WED</v>
+        <v>FRI</v>
       </c>
       <c r="AG70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>THU</v>
+        <v>SAT</v>
       </c>
       <c r="AH70" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>FRI</v>
+        <v>SUN</v>
       </c>
     </row>
     <row r="71" spans="4:34" x14ac:dyDescent="0.3">
@@ -12965,123 +12949,123 @@
     <row r="72" spans="4:34" x14ac:dyDescent="0.3">
       <c r="E72" t="str">
         <f ca="1">TEXT(E55,"dd")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" ref="F72:AH72" ca="1" si="24">TEXT(F55,"dd")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>27</v>
+        <v>01</v>
       </c>
       <c r="Q72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>28</v>
+        <v>02</v>
       </c>
       <c r="R72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>01</v>
+        <v>03</v>
       </c>
       <c r="S72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="T72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>03</v>
+        <v>05</v>
       </c>
       <c r="U72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>04</v>
+        <v>06</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>05</v>
+        <v>07</v>
       </c>
       <c r="W72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>06</v>
+        <v>08</v>
       </c>
       <c r="X72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>07</v>
+        <v>09</v>
       </c>
       <c r="Y72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>08</v>
+        <v>10</v>
       </c>
       <c r="Z72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>09</v>
+        <v>11</v>
       </c>
       <c r="AA72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AC72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AD72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AE72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AF72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AG72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AH72" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -13092,6 +13076,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -13302,14 +13294,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13320,6 +13304,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5BB6EA-B4A9-4FD0-A581-32FE787E0D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13338,16 +13332,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
   <ds:schemaRefs>

</xml_diff>